<commit_message>
Update: Advancement.xlsx File from Crowdin
</commit_message>
<xml_diff>
--- a/ja/Advancement.xlsx
+++ b/ja/Advancement.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>日本語</t>
   </si>
@@ -88,6 +88,9 @@
     <t>Avanzamento</t>
   </si>
   <si>
+    <t>발전 과제</t>
+  </si>
+  <si>
     <t>Avanço</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t xml:space="preserve">Stato avanzamento </t>
   </si>
   <si>
+    <t>발전 과제 상태를 확인하세요.</t>
+  </si>
+  <si>
     <t>Status de Avanço</t>
   </si>
   <si>
@@ -136,6 +142,9 @@
     <t>Avanzamento Completato</t>
   </si>
   <si>
+    <t>발전 과제 완료</t>
+  </si>
+  <si>
     <t>Progresso Concluído</t>
   </si>
   <si>
@@ -160,6 +169,9 @@
     <t>Nome Avanzamento</t>
   </si>
   <si>
+    <t>발전 과제 이름</t>
+  </si>
+  <si>
     <t>Nome do Avanço</t>
   </si>
   <si>
@@ -184,6 +196,9 @@
     <t>Tempo avanzamento</t>
   </si>
   <si>
+    <t>완료일</t>
+  </si>
+  <si>
     <t>Tempo do Avanço</t>
   </si>
   <si>
@@ -206,6 +221,9 @@
   </si>
   <si>
     <t>Progresso avanzamento</t>
+  </si>
+  <si>
+    <t>발전 과제 진행 상황</t>
   </si>
   <si>
     <t>Progresso do Avanço</t>
@@ -700,148 +718,166 @@
       <c r="H2" t="s">
         <v>24</v>
       </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="V3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="P4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="V4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="P5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="V5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
+        <v>61</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="O6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="V6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>70</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="O7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P7" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="V7" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>